<commit_message>
Tuned new equilibria for low endemicity
</commit_message>
<xml_diff>
--- a/Zetas_ICL_func.xlsx
+++ b/Zetas_ICL_func.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z541213\Documents\Project\Model\Schisto_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE29607-8788-42BA-8B9B-EB4B272917D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EC4882-6CAA-46DF-ACD6-D509CFA84A84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="16">
   <si>
     <t xml:space="preserve">Endemicity </t>
   </si>
@@ -77,17 +77,24 @@
   <si>
     <t>Transmission on snails</t>
   </si>
+  <si>
+    <t>Equilibrium</t>
+  </si>
+  <si>
+    <t>TRUE?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0E+00"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +106,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -264,7 +278,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -277,6 +290,11 @@
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,11 +575,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFC76"/>
+  <dimension ref="A1:XFC82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,6 +588,7 @@
     <col min="5" max="5" width="14.88671875" customWidth="1"/>
     <col min="6" max="6" width="17.44140625" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -597,6 +616,9 @@
       <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
@@ -614,7 +636,9 @@
       <c r="E2" s="3">
         <v>0</v>
       </c>
-      <c r="I2"/>
+      <c r="I2" s="54" t="b">
+        <v>0</v>
+      </c>
       <c r="J2"/>
       <c r="K2"/>
       <c r="L2"/>
@@ -656,7 +680,9 @@
       <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="I3"/>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
       <c r="J3"/>
       <c r="K3"/>
       <c r="L3"/>
@@ -698,7 +724,9 @@
       <c r="H4" s="4">
         <v>0</v>
       </c>
-      <c r="I4"/>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -739,7 +767,9 @@
       <c r="H5" s="6">
         <v>0</v>
       </c>
-      <c r="I5"/>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5"/>
@@ -780,7 +810,9 @@
       <c r="H6" s="6">
         <v>0</v>
       </c>
-      <c r="I6"/>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
@@ -821,7 +853,9 @@
       <c r="H7" s="6">
         <v>0</v>
       </c>
-      <c r="I7"/>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -862,7 +896,9 @@
       <c r="H8" s="8">
         <v>0</v>
       </c>
-      <c r="I8"/>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
@@ -903,7 +939,9 @@
       <c r="H9" s="8">
         <v>0</v>
       </c>
-      <c r="I9"/>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9"/>
@@ -944,7 +982,9 @@
       <c r="H10" s="8">
         <v>0</v>
       </c>
-      <c r="I10"/>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10"/>
@@ -986,7 +1026,9 @@
         <f>3*10^(-10)</f>
         <v>3E-10</v>
       </c>
-      <c r="I11"/>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11"/>
@@ -1028,7 +1070,9 @@
         <f>3.2*10^(-10)</f>
         <v>3.2000000000000003E-10</v>
       </c>
-      <c r="I12"/>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
       <c r="J12"/>
       <c r="K12"/>
       <c r="L12"/>
@@ -1070,7 +1114,9 @@
         <f>3.2*10^(-10)</f>
         <v>3.2000000000000003E-10</v>
       </c>
-      <c r="I13"/>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
       <c r="J13"/>
       <c r="K13"/>
       <c r="L13"/>
@@ -1111,7 +1157,9 @@
       <c r="H14" s="12">
         <v>3E-10</v>
       </c>
-      <c r="I14"/>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
       <c r="J14"/>
       <c r="K14"/>
       <c r="L14"/>
@@ -1152,7 +1200,9 @@
       <c r="H15" s="12">
         <v>3E-10</v>
       </c>
-      <c r="I15"/>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
       <c r="J15"/>
       <c r="K15"/>
       <c r="L15"/>
@@ -1193,7 +1243,9 @@
       <c r="H16" s="12">
         <v>3E-10</v>
       </c>
-      <c r="I16"/>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
       <c r="J16"/>
       <c r="K16"/>
       <c r="L16"/>
@@ -1234,7 +1286,9 @@
       <c r="H17" s="14">
         <v>4.0000000000000001E-10</v>
       </c>
-      <c r="I17"/>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
       <c r="J17"/>
       <c r="K17"/>
       <c r="L17"/>
@@ -1275,7 +1329,9 @@
       <c r="H18" s="14">
         <v>4.0000000000000001E-10</v>
       </c>
-      <c r="I18"/>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
       <c r="J18"/>
       <c r="K18"/>
       <c r="L18"/>
@@ -1316,7 +1372,9 @@
       <c r="H19" s="14">
         <v>4.0000000000000001E-10</v>
       </c>
-      <c r="I19"/>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
       <c r="J19"/>
       <c r="K19"/>
       <c r="L19"/>
@@ -1354,10 +1412,12 @@
       <c r="G20" s="16">
         <v>0.15</v>
       </c>
-      <c r="H20" s="47">
+      <c r="H20" s="46">
         <v>3.7999999999999998E-10</v>
       </c>
-      <c r="I20"/>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
@@ -1395,10 +1455,12 @@
       <c r="G21" s="16">
         <v>0.15</v>
       </c>
-      <c r="H21" s="41">
+      <c r="H21" s="40">
         <v>4.0000000000000001E-10</v>
       </c>
-      <c r="I21"/>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
       <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
@@ -1436,10 +1498,12 @@
       <c r="G22" s="16">
         <v>0.15</v>
       </c>
-      <c r="H22" s="41">
+      <c r="H22" s="40">
         <v>4.0000000000000001E-10</v>
       </c>
-      <c r="I22"/>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
       <c r="J22"/>
       <c r="K22"/>
       <c r="L22"/>
@@ -1477,10 +1541,12 @@
       <c r="G23" s="18">
         <v>0.15</v>
       </c>
-      <c r="H23" s="42">
+      <c r="H23" s="41">
         <v>3E-10</v>
       </c>
-      <c r="I23"/>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
       <c r="J23"/>
       <c r="K23"/>
       <c r="L23"/>
@@ -1518,10 +1584,12 @@
       <c r="G24" s="18">
         <v>0.15</v>
       </c>
-      <c r="H24" s="42">
+      <c r="H24" s="41">
         <v>4.0000000000000001E-10</v>
       </c>
-      <c r="I24"/>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
       <c r="J24"/>
       <c r="K24"/>
       <c r="L24"/>
@@ -1559,10 +1627,12 @@
       <c r="G25" s="18">
         <v>0.15</v>
       </c>
-      <c r="H25" s="42">
+      <c r="H25" s="41">
         <v>4.0000000000000001E-10</v>
       </c>
-      <c r="I25"/>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
       <c r="J25"/>
       <c r="K25"/>
       <c r="L25"/>
@@ -1600,10 +1670,12 @@
       <c r="G26" s="20">
         <v>0.12</v>
       </c>
-      <c r="H26" s="40">
+      <c r="H26" s="39">
         <v>4.0000000000000001E-10</v>
       </c>
-      <c r="I26"/>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
       <c r="J26"/>
       <c r="K26"/>
       <c r="L26"/>
@@ -1641,10 +1713,12 @@
       <c r="G27" s="20">
         <v>0.12</v>
       </c>
-      <c r="H27" s="40">
+      <c r="H27" s="39">
         <v>4.0000000000000001E-10</v>
       </c>
-      <c r="I27"/>
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
       <c r="J27"/>
       <c r="K27"/>
       <c r="L27"/>
@@ -1682,10 +1756,12 @@
       <c r="G28" s="26">
         <v>0.12</v>
       </c>
-      <c r="H28" s="43">
+      <c r="H28" s="42">
         <v>4.0000000000000001E-10</v>
       </c>
-      <c r="I28"/>
+      <c r="I28" s="51" t="b">
+        <v>1</v>
+      </c>
       <c r="J28"/>
       <c r="K28"/>
       <c r="L28"/>
@@ -1720,6 +1796,9 @@
       <c r="F29" s="2"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
+      <c r="I29" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="29" t="s">
@@ -1737,7 +1816,7 @@
       <c r="E30" s="5">
         <v>0</v>
       </c>
-      <c r="F30" s="49">
+      <c r="F30" s="48">
         <v>9.5000000000000005E-5</v>
       </c>
       <c r="G30" s="4">
@@ -1745,6 +1824,9 @@
       </c>
       <c r="H30" s="4">
         <v>0</v>
+      </c>
+      <c r="I30" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
@@ -1772,6 +1854,9 @@
       <c r="H31" s="4">
         <v>0</v>
       </c>
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="30" t="s">
@@ -1799,6 +1884,9 @@
       <c r="H32" s="6">
         <v>0</v>
       </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A33" s="30" t="s">
@@ -1826,6 +1914,9 @@
       <c r="H33" s="6">
         <v>0</v>
       </c>
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A34" s="30" t="s">
@@ -1853,6 +1944,9 @@
       <c r="H34" s="6">
         <v>0</v>
       </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A35" s="31" t="s">
@@ -1880,6 +1974,9 @@
       <c r="H35" s="8">
         <v>0</v>
       </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
@@ -1907,6 +2004,9 @@
       <c r="H36" s="8">
         <v>0</v>
       </c>
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
@@ -1934,6 +2034,9 @@
       <c r="H37" s="8">
         <v>0</v>
       </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:16383" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="36" t="s">
@@ -1961,7 +2064,9 @@
         <f>9*10^(-11)</f>
         <v>8.9999999999999999E-11</v>
       </c>
-      <c r="I38"/>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
       <c r="J38"/>
       <c r="K38"/>
       <c r="L38"/>
@@ -2001,7 +2106,9 @@
         <f>9*10^(-11)</f>
         <v>8.9999999999999999E-11</v>
       </c>
-      <c r="I39"/>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
       <c r="J39"/>
       <c r="K39"/>
       <c r="L39"/>
@@ -2041,7 +2148,9 @@
         <f>9*10^(-11)</f>
         <v>8.9999999999999999E-11</v>
       </c>
-      <c r="I40"/>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
       <c r="J40"/>
       <c r="K40"/>
       <c r="L40"/>
@@ -2080,7 +2189,9 @@
       <c r="H41" s="12">
         <v>1E-10</v>
       </c>
-      <c r="I41"/>
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
       <c r="J41"/>
       <c r="K41"/>
       <c r="L41"/>
@@ -2119,7 +2230,9 @@
       <c r="H42" s="12">
         <v>1E-10</v>
       </c>
-      <c r="I42"/>
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
       <c r="J42"/>
       <c r="K42"/>
       <c r="L42"/>
@@ -2158,7 +2271,9 @@
       <c r="H43" s="12">
         <v>1E-10</v>
       </c>
-      <c r="I43"/>
+      <c r="I43" t="b">
+        <v>1</v>
+      </c>
       <c r="J43"/>
       <c r="K43"/>
       <c r="L43"/>
@@ -2197,7 +2312,9 @@
       <c r="H44" s="14">
         <v>1.2999999999999999E-10</v>
       </c>
-      <c r="I44"/>
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
       <c r="J44"/>
       <c r="K44"/>
       <c r="L44"/>
@@ -2236,7 +2353,9 @@
       <c r="H45" s="14">
         <v>1.2999999999999999E-10</v>
       </c>
-      <c r="I45"/>
+      <c r="I45" t="b">
+        <v>1</v>
+      </c>
       <c r="J45"/>
       <c r="K45"/>
       <c r="L45"/>
@@ -2275,7 +2394,9 @@
       <c r="H46" s="14">
         <v>1.2999999999999999E-10</v>
       </c>
-      <c r="I46"/>
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
       <c r="J46"/>
       <c r="K46"/>
       <c r="L46"/>
@@ -2313,6 +2434,9 @@
       </c>
       <c r="H47" s="16">
         <v>1E-10</v>
+      </c>
+      <c r="I47" t="b">
+        <v>1</v>
       </c>
       <c r="V47" s="16"/>
       <c r="W47" s="16"/>
@@ -18702,6 +18826,9 @@
       <c r="H48" s="16">
         <v>8.9999999999999999E-11</v>
       </c>
+      <c r="I48" t="b">
+        <v>1</v>
+      </c>
       <c r="V48" s="16"/>
       <c r="W48" s="16"/>
       <c r="X48" s="16"/>
@@ -35090,6 +35217,9 @@
       <c r="H49" s="16">
         <v>8.9999999999999999E-11</v>
       </c>
+      <c r="I49" t="b">
+        <v>1</v>
+      </c>
       <c r="V49" s="16"/>
       <c r="W49" s="16"/>
       <c r="X49" s="16"/>
@@ -51478,6 +51608,9 @@
       <c r="H50" s="18">
         <v>8.9999999999999999E-11</v>
       </c>
+      <c r="I50" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A51" s="33" t="s">
@@ -51504,6 +51637,9 @@
       <c r="H51" s="18">
         <v>8.9999999999999999E-11</v>
       </c>
+      <c r="I51" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A52" s="33" t="s">
@@ -51530,6 +51666,9 @@
       <c r="H52" s="18">
         <v>8.9999999999999999E-11</v>
       </c>
+      <c r="I52" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A53" s="34" t="s">
@@ -51553,8 +51692,11 @@
       <c r="G53" s="20">
         <v>0.26</v>
       </c>
-      <c r="H53" s="50">
+      <c r="H53" s="49">
         <v>1.2999999999999999E-10</v>
+      </c>
+      <c r="I53" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51579,8 +51721,11 @@
       <c r="G54" s="20">
         <v>0.26</v>
       </c>
-      <c r="H54" s="50">
+      <c r="H54" s="49">
         <v>1.2999999999999999E-10</v>
+      </c>
+      <c r="I54" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:16383" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -51605,357 +51750,303 @@
       <c r="G55" s="26">
         <v>0.26</v>
       </c>
-      <c r="H55" s="51">
+      <c r="H55" s="50">
         <v>1.2999999999999999E-10</v>
+      </c>
+      <c r="I55" s="51" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:16383" x14ac:dyDescent="0.3">
-      <c r="A56" s="39" t="s">
+      <c r="A56" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B56" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="8" t="s">
+      <c r="B56" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="C56" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E56" s="9">
+      <c r="D56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E56" s="3">
         <v>0</v>
       </c>
-      <c r="F56" s="8">
-        <v>8.2000000000000001E-5</v>
-      </c>
-      <c r="G56" s="8">
+      <c r="F56" s="55">
+        <v>7.8499999999999997E-5</v>
+      </c>
+      <c r="G56" s="4">
         <v>0.1</v>
       </c>
-      <c r="H56" s="8">
+      <c r="H56" s="4">
+        <v>0</v>
+      </c>
+      <c r="I56" s="54" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:16383" x14ac:dyDescent="0.3">
-      <c r="A57" s="31" t="s">
+      <c r="A57" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B57" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" s="8" t="s">
+      <c r="B57" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="C57" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="9">
+      <c r="E57" s="5">
         <v>0</v>
       </c>
-      <c r="F57" s="8">
-        <v>8.2000000000000001E-5</v>
-      </c>
-      <c r="G57" s="8">
+      <c r="F57" s="55">
+        <v>7.7799999999999994E-5</v>
+      </c>
+      <c r="G57" s="4">
         <v>0.1</v>
       </c>
-      <c r="H57" s="8">
+      <c r="H57" s="4">
         <v>0</v>
+      </c>
+      <c r="I57" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:16383" x14ac:dyDescent="0.3">
-      <c r="A58" s="31" t="s">
+      <c r="A58" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="E58" s="5">
+        <v>0</v>
+      </c>
+      <c r="F58" s="55">
+        <v>7.7700000000000005E-5</v>
+      </c>
+      <c r="G58" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H58" s="4">
+        <v>0</v>
+      </c>
+      <c r="I58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16383" x14ac:dyDescent="0.3">
+      <c r="A59" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="8" t="s">
+      <c r="D59" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="7">
+        <v>0</v>
+      </c>
+      <c r="F59" s="53">
+        <v>7.8999999999999996E-5</v>
+      </c>
+      <c r="G59" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H59" s="6">
+        <v>0</v>
+      </c>
+      <c r="I59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16383" x14ac:dyDescent="0.3">
+      <c r="A60" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="7">
+        <v>0</v>
+      </c>
+      <c r="F60" s="52">
+        <v>7.8499999999999997E-5</v>
+      </c>
+      <c r="G60" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H60" s="6">
+        <v>0</v>
+      </c>
+      <c r="I60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16383" x14ac:dyDescent="0.3">
+      <c r="A61" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E58" s="9">
+      <c r="E61" s="7">
         <v>0</v>
       </c>
-      <c r="F58" s="8">
+      <c r="F61" s="52">
+        <v>7.8499999999999997E-5</v>
+      </c>
+      <c r="G61" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H61" s="6">
+        <v>0</v>
+      </c>
+      <c r="I61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16383" x14ac:dyDescent="0.3">
+      <c r="A62" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" s="9">
+        <v>0</v>
+      </c>
+      <c r="F62" s="8">
         <v>8.2000000000000001E-5</v>
       </c>
-      <c r="G58" s="8">
+      <c r="G62" s="8">
         <v>0.1</v>
       </c>
-      <c r="H58" s="8">
+      <c r="H62" s="8">
         <v>0</v>
       </c>
+      <c r="I62" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="59" spans="1:16383" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="36" t="s">
+    <row r="63" spans="1:16383" x14ac:dyDescent="0.3">
+      <c r="A63" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B63" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="D63" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D59" s="10" t="s">
+      <c r="E63" s="9">
+        <v>0</v>
+      </c>
+      <c r="F63" s="8">
+        <v>8.2000000000000001E-5</v>
+      </c>
+      <c r="G63" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="H63" s="8">
+        <v>0</v>
+      </c>
+      <c r="I63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16383" x14ac:dyDescent="0.3">
+      <c r="A64" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E59" s="11">
+      <c r="D64" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="9">
+        <v>0</v>
+      </c>
+      <c r="F64" s="8">
+        <v>8.2000000000000001E-5</v>
+      </c>
+      <c r="G64" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="H64" s="8">
+        <v>0</v>
+      </c>
+      <c r="I64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" s="11">
         <v>0.06</v>
       </c>
-      <c r="F59" s="10">
+      <c r="F65" s="10">
         <v>9.7999999999999997E-4</v>
       </c>
-      <c r="G59" s="10">
+      <c r="G65" s="10">
         <v>0.1</v>
       </c>
-      <c r="H59" s="44">
+      <c r="H65" s="43">
         <f>0.000000004</f>
         <v>4.0000000000000002E-9</v>
       </c>
-      <c r="I59"/>
-      <c r="J59"/>
-      <c r="K59"/>
-      <c r="L59"/>
-      <c r="M59"/>
-      <c r="N59"/>
-      <c r="O59"/>
-      <c r="P59"/>
-      <c r="Q59"/>
-      <c r="R59"/>
-      <c r="S59"/>
-      <c r="T59"/>
-      <c r="U59"/>
-      <c r="V59"/>
-    </row>
-    <row r="60" spans="1:16383" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E60" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F60" s="10">
-        <v>9.7999999999999997E-4</v>
-      </c>
-      <c r="G60" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="H60" s="44">
-        <f>0.000000005*0.8</f>
-        <v>4.0000000000000002E-9</v>
-      </c>
-      <c r="I60"/>
-      <c r="J60"/>
-      <c r="K60"/>
-      <c r="L60"/>
-      <c r="M60"/>
-      <c r="N60"/>
-      <c r="O60"/>
-      <c r="P60"/>
-      <c r="Q60"/>
-      <c r="R60"/>
-      <c r="S60"/>
-      <c r="T60"/>
-      <c r="U60"/>
-      <c r="V60"/>
-    </row>
-    <row r="61" spans="1:16383" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E61" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F61" s="10">
-        <v>9.7999999999999997E-4</v>
-      </c>
-      <c r="G61" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="H61" s="44">
-        <f>0.000000005*0.8</f>
-        <v>4.0000000000000002E-9</v>
-      </c>
-      <c r="I61"/>
-      <c r="J61"/>
-      <c r="K61"/>
-      <c r="L61"/>
-      <c r="M61"/>
-      <c r="N61"/>
-      <c r="O61"/>
-      <c r="P61"/>
-      <c r="Q61"/>
-      <c r="R61"/>
-      <c r="S61"/>
-      <c r="T61"/>
-      <c r="U61"/>
-      <c r="V61"/>
-    </row>
-    <row r="62" spans="1:16383" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E62" s="13">
-        <v>0.06</v>
-      </c>
-      <c r="F62" s="12">
-        <v>9.8999999999999999E-4</v>
-      </c>
-      <c r="G62" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="H62" s="45">
-        <v>4.0000000000000002E-9</v>
-      </c>
-      <c r="I62"/>
-      <c r="J62"/>
-      <c r="K62"/>
-      <c r="L62"/>
-      <c r="M62"/>
-      <c r="N62"/>
-      <c r="O62"/>
-      <c r="P62"/>
-      <c r="Q62"/>
-      <c r="R62"/>
-      <c r="S62"/>
-      <c r="T62"/>
-      <c r="U62"/>
-      <c r="V62"/>
-    </row>
-    <row r="63" spans="1:16383" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E63" s="13">
-        <v>0.06</v>
-      </c>
-      <c r="F63" s="12">
-        <v>9.8999999999999999E-4</v>
-      </c>
-      <c r="G63" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="H63" s="45">
-        <v>4.0000000000000002E-9</v>
-      </c>
-      <c r="I63"/>
-      <c r="J63"/>
-      <c r="K63"/>
-      <c r="L63"/>
-      <c r="M63"/>
-      <c r="N63"/>
-      <c r="O63"/>
-      <c r="P63"/>
-      <c r="Q63"/>
-      <c r="R63"/>
-      <c r="S63"/>
-      <c r="T63"/>
-      <c r="U63"/>
-      <c r="V63"/>
-    </row>
-    <row r="64" spans="1:16383" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C64" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E64" s="13">
-        <v>0.06</v>
-      </c>
-      <c r="F64" s="12">
-        <v>9.8999999999999999E-4</v>
-      </c>
-      <c r="G64" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="H64" s="45">
-        <v>4.0000000000000002E-9</v>
-      </c>
-      <c r="I64"/>
-      <c r="J64"/>
-      <c r="K64"/>
-      <c r="L64"/>
-      <c r="M64"/>
-      <c r="N64"/>
-      <c r="O64"/>
-      <c r="P64"/>
-      <c r="Q64"/>
-      <c r="R64"/>
-      <c r="S64"/>
-      <c r="T64"/>
-      <c r="U64"/>
-      <c r="V64"/>
-    </row>
-    <row r="65" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E65" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="F65" s="14">
-        <v>1E-3</v>
-      </c>
-      <c r="G65" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="H65" s="46">
-        <v>4.0000000000000002E-9</v>
-      </c>
-      <c r="I65"/>
+      <c r="I65" t="b">
+        <v>1</v>
+      </c>
       <c r="J65"/>
       <c r="K65"/>
       <c r="L65"/>
@@ -51970,32 +52061,35 @@
       <c r="U65"/>
       <c r="V65"/>
     </row>
-    <row r="66" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="38" t="s">
+    <row r="66" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B66" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" s="14" t="s">
+      <c r="B66" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D66" s="14" t="s">
+      <c r="D66" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E66" s="15">
+      <c r="E66" s="11">
         <v>0.06</v>
       </c>
-      <c r="F66" s="14">
-        <v>1E-3</v>
-      </c>
-      <c r="G66" s="14">
+      <c r="F66" s="10">
+        <v>9.7999999999999997E-4</v>
+      </c>
+      <c r="G66" s="10">
         <v>0.1</v>
       </c>
-      <c r="H66" s="46">
+      <c r="H66" s="43">
+        <f>0.000000005*0.8</f>
         <v>4.0000000000000002E-9</v>
       </c>
-      <c r="I66"/>
+      <c r="I66" t="b">
+        <v>1</v>
+      </c>
       <c r="J66"/>
       <c r="K66"/>
       <c r="L66"/>
@@ -52010,32 +52104,35 @@
       <c r="U66"/>
       <c r="V66"/>
     </row>
-    <row r="67" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="38" t="s">
+    <row r="67" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C67" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E67" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="F67" s="14">
-        <v>1E-3</v>
-      </c>
-      <c r="G67" s="14">
+      <c r="E67" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F67" s="10">
+        <v>9.7999999999999997E-4</v>
+      </c>
+      <c r="G67" s="10">
         <v>0.1</v>
       </c>
-      <c r="H67" s="46">
+      <c r="H67" s="43">
+        <f>0.000000005*0.8</f>
         <v>4.0000000000000002E-9</v>
       </c>
-      <c r="I67"/>
+      <c r="I67" t="b">
+        <v>1</v>
+      </c>
       <c r="J67"/>
       <c r="K67"/>
       <c r="L67"/>
@@ -52050,241 +52147,520 @@
       <c r="U67"/>
       <c r="V67"/>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A68" s="32" t="s">
+    <row r="68" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B68" s="24" t="s">
+      <c r="B68" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C68" s="24" t="s">
+      <c r="E68" s="13">
+        <v>0.06</v>
+      </c>
+      <c r="F68" s="12">
+        <v>9.8999999999999999E-4</v>
+      </c>
+      <c r="G68" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="H68" s="44">
+        <v>4.0000000000000002E-9</v>
+      </c>
+      <c r="I68" t="b">
+        <v>1</v>
+      </c>
+      <c r="J68"/>
+      <c r="K68"/>
+      <c r="L68"/>
+      <c r="M68"/>
+      <c r="N68"/>
+      <c r="O68"/>
+      <c r="P68"/>
+      <c r="Q68"/>
+      <c r="R68"/>
+      <c r="S68"/>
+      <c r="T68"/>
+      <c r="U68"/>
+      <c r="V68"/>
+    </row>
+    <row r="69" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" s="13">
+        <v>0.06</v>
+      </c>
+      <c r="F69" s="12">
+        <v>9.8999999999999999E-4</v>
+      </c>
+      <c r="G69" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="H69" s="44">
+        <v>4.0000000000000002E-9</v>
+      </c>
+      <c r="I69" t="b">
+        <v>1</v>
+      </c>
+      <c r="J69"/>
+      <c r="K69"/>
+      <c r="L69"/>
+      <c r="M69"/>
+      <c r="N69"/>
+      <c r="O69"/>
+      <c r="P69"/>
+      <c r="Q69"/>
+      <c r="R69"/>
+      <c r="S69"/>
+      <c r="T69"/>
+      <c r="U69"/>
+      <c r="V69"/>
+    </row>
+    <row r="70" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="24" t="s">
+      <c r="E70" s="13">
+        <v>0.06</v>
+      </c>
+      <c r="F70" s="12">
+        <v>9.8999999999999999E-4</v>
+      </c>
+      <c r="G70" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="H70" s="44">
+        <v>4.0000000000000002E-9</v>
+      </c>
+      <c r="I70" t="b">
+        <v>1</v>
+      </c>
+      <c r="J70"/>
+      <c r="K70"/>
+      <c r="L70"/>
+      <c r="M70"/>
+      <c r="N70"/>
+      <c r="O70"/>
+      <c r="P70"/>
+      <c r="Q70"/>
+      <c r="R70"/>
+      <c r="S70"/>
+      <c r="T70"/>
+      <c r="U70"/>
+      <c r="V70"/>
+    </row>
+    <row r="71" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E68" s="25">
+      <c r="E71" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="F71" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="G71" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="H71" s="45">
+        <v>4.0000000000000002E-9</v>
+      </c>
+      <c r="I71" t="b">
+        <v>1</v>
+      </c>
+      <c r="J71"/>
+      <c r="K71"/>
+      <c r="L71"/>
+      <c r="M71"/>
+      <c r="N71"/>
+      <c r="O71"/>
+      <c r="P71"/>
+      <c r="Q71"/>
+      <c r="R71"/>
+      <c r="S71"/>
+      <c r="T71"/>
+      <c r="U71"/>
+      <c r="V71"/>
+    </row>
+    <row r="72" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" s="15">
         <v>0.06</v>
       </c>
-      <c r="F68" s="24">
+      <c r="F72" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="G72" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="H72" s="45">
+        <v>4.0000000000000002E-9</v>
+      </c>
+      <c r="I72" t="b">
+        <v>1</v>
+      </c>
+      <c r="J72"/>
+      <c r="K72"/>
+      <c r="L72"/>
+      <c r="M72"/>
+      <c r="N72"/>
+      <c r="O72"/>
+      <c r="P72"/>
+      <c r="Q72"/>
+      <c r="R72"/>
+      <c r="S72"/>
+      <c r="T72"/>
+      <c r="U72"/>
+      <c r="V72"/>
+    </row>
+    <row r="73" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="F73" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="G73" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="H73" s="45">
+        <v>4.0000000000000002E-9</v>
+      </c>
+      <c r="I73" t="b">
+        <v>1</v>
+      </c>
+      <c r="J73"/>
+      <c r="K73"/>
+      <c r="L73"/>
+      <c r="M73"/>
+      <c r="N73"/>
+      <c r="O73"/>
+      <c r="P73"/>
+      <c r="Q73"/>
+      <c r="R73"/>
+      <c r="S73"/>
+      <c r="T73"/>
+      <c r="U73"/>
+      <c r="V73"/>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A74" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B74" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E74" s="25">
+        <v>0.06</v>
+      </c>
+      <c r="F74" s="24">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="G68" s="24">
+      <c r="G74" s="24">
         <v>0.1</v>
       </c>
-      <c r="H68" s="47">
+      <c r="H74" s="46">
         <f>0.0000000045*0.8</f>
         <v>3.6E-9</v>
       </c>
+      <c r="I74" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A69" s="32" t="s">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A75" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B69" s="16" t="s">
+      <c r="B75" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C69" s="16" t="s">
+      <c r="C75" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D69" s="16" t="s">
+      <c r="D75" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E69" s="25">
+      <c r="E75" s="25">
         <v>0.06</v>
       </c>
-      <c r="F69" s="24">
+      <c r="F75" s="24">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="G69" s="24">
+      <c r="G75" s="24">
         <v>0.1</v>
       </c>
-      <c r="H69" s="47">
-        <f t="shared" ref="H69:H70" si="0">0.0000000045*0.8</f>
+      <c r="H75" s="46">
+        <f t="shared" ref="H75:H76" si="0">0.0000000045*0.8</f>
         <v>3.6E-9</v>
       </c>
+      <c r="I75" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A70" s="32" t="s">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A76" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B70" s="24" t="s">
+      <c r="B76" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="24" t="s">
+      <c r="C76" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D70" s="24" t="s">
+      <c r="D76" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E70" s="25">
+      <c r="E76" s="25">
         <v>0.06</v>
       </c>
-      <c r="F70" s="24">
+      <c r="F76" s="24">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="G70" s="24">
+      <c r="G76" s="24">
         <v>0.1</v>
       </c>
-      <c r="H70" s="47">
+      <c r="H76" s="46">
         <f t="shared" si="0"/>
         <v>3.6E-9</v>
       </c>
+      <c r="I76" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A71" s="33" t="s">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A77" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B71" s="18" t="s">
+      <c r="B77" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C71" s="18" t="s">
+      <c r="C77" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D71" s="18" t="s">
+      <c r="D77" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E71" s="19">
+      <c r="E77" s="19">
         <v>0.06</v>
       </c>
-      <c r="F71" s="18">
+      <c r="F77" s="18">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="G71" s="18">
+      <c r="G77" s="18">
         <v>0.1</v>
       </c>
-      <c r="H71" s="48">
+      <c r="H77" s="47">
         <v>3.6E-9</v>
       </c>
+      <c r="I77" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A72" s="33" t="s">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A78" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B72" s="18" t="s">
+      <c r="B78" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C72" s="18" t="s">
+      <c r="C78" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D72" s="18" t="s">
+      <c r="D78" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E72" s="19">
+      <c r="E78" s="19">
         <v>0.06</v>
       </c>
-      <c r="F72" s="18">
+      <c r="F78" s="18">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="G72" s="18">
+      <c r="G78" s="18">
         <v>0.1</v>
       </c>
-      <c r="H72" s="48">
+      <c r="H78" s="47">
         <v>3.6E-9</v>
       </c>
+      <c r="I78" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A73" s="33" t="s">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A79" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B73" s="18" t="s">
+      <c r="B79" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C73" s="18" t="s">
+      <c r="C79" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D73" s="18" t="s">
+      <c r="D79" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E73" s="19">
+      <c r="E79" s="19">
         <v>0.06</v>
       </c>
-      <c r="F73" s="18">
+      <c r="F79" s="18">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="G73" s="18">
+      <c r="G79" s="18">
         <v>0.1</v>
       </c>
-      <c r="H73" s="48">
+      <c r="H79" s="47">
         <v>3.6E-9</v>
       </c>
+      <c r="I79" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A74" s="34" t="s">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A80" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B74" s="20" t="s">
+      <c r="B80" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C74" s="20" t="s">
+      <c r="C80" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D74" s="20" t="s">
+      <c r="D80" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E74" s="21">
+      <c r="E80" s="21">
         <v>0.05</v>
       </c>
-      <c r="F74" s="20">
+      <c r="F80" s="20">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="G74" s="20">
+      <c r="G80" s="20">
         <v>0.1</v>
       </c>
-      <c r="H74" s="20">
+      <c r="H80" s="20">
         <v>3.6E-9</v>
       </c>
+      <c r="I80" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A75" s="34" t="s">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B75" s="20" t="s">
+      <c r="B81" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C75" s="20" t="s">
+      <c r="C81" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D75" s="20" t="s">
+      <c r="D81" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="21">
+      <c r="E81" s="21">
         <v>0.05</v>
       </c>
-      <c r="F75" s="20">
+      <c r="F81" s="20">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="G75" s="20">
+      <c r="G81" s="20">
         <v>0.1</v>
       </c>
-      <c r="H75" s="20">
+      <c r="H81" s="20">
         <v>3.6E-9</v>
       </c>
+      <c r="I81" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="35" t="s">
+    <row r="82" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B76" s="26" t="s">
+      <c r="B82" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C76" s="26" t="s">
+      <c r="C82" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D76" s="26" t="s">
+      <c r="D82" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E76" s="27">
+      <c r="E82" s="27">
         <v>0.05</v>
       </c>
-      <c r="F76" s="26">
+      <c r="F82" s="26">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="G76" s="26">
+      <c r="G82" s="26">
         <v>0.1</v>
       </c>
-      <c r="H76" s="26">
+      <c r="H82" s="26">
         <v>3.6E-9</v>
+      </c>
+      <c r="I82" s="51" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted zetas - low equilibria
</commit_message>
<xml_diff>
--- a/Zetas_ICL_func.xlsx
+++ b/Zetas_ICL_func.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z541213\Documents\Project\Model\Schisto_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EC4882-6CAA-46DF-ACD6-D509CFA84A84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC830436-6231-4DED-9DD1-0B1CEADBB9C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="15">
   <si>
     <t xml:space="preserve">Endemicity </t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Equilibrium</t>
-  </si>
-  <si>
-    <t>TRUE?</t>
   </si>
 </sst>
 </file>
@@ -579,7 +576,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I59" sqref="I59"/>
+      <selection pane="bottomLeft" activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51811,8 +51808,8 @@
       <c r="H57" s="4">
         <v>0</v>
       </c>
-      <c r="I57" t="s">
-        <v>15</v>
+      <c r="I57" s="54" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51840,8 +51837,8 @@
       <c r="H58" s="4">
         <v>0</v>
       </c>
-      <c r="I58" t="s">
-        <v>15</v>
+      <c r="I58" s="54" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51869,8 +51866,8 @@
       <c r="H59" s="6">
         <v>0</v>
       </c>
-      <c r="I59" t="b">
-        <v>1</v>
+      <c r="I59" s="54" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51898,8 +51895,8 @@
       <c r="H60" s="6">
         <v>0</v>
       </c>
-      <c r="I60" t="b">
-        <v>1</v>
+      <c r="I60" s="54" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51927,8 +51924,8 @@
       <c r="H61" s="6">
         <v>0</v>
       </c>
-      <c r="I61" t="b">
-        <v>1</v>
+      <c r="I61" s="54" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51956,8 +51953,8 @@
       <c r="H62" s="8">
         <v>0</v>
       </c>
-      <c r="I62" t="b">
-        <v>1</v>
+      <c r="I62" s="54" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51985,8 +51982,8 @@
       <c r="H63" s="8">
         <v>0</v>
       </c>
-      <c r="I63" t="b">
-        <v>1</v>
+      <c r="I63" s="54" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:16383" x14ac:dyDescent="0.3">
@@ -52014,8 +52011,8 @@
       <c r="H64" s="8">
         <v>0</v>
       </c>
-      <c r="I64" t="b">
-        <v>1</v>
+      <c r="I64" s="54" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added mean intensity to population output
</commit_message>
<xml_diff>
--- a/Zetas_ICL_func.xlsx
+++ b/Zetas_ICL_func.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z541213\Documents\Project\Model\Schisto_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z541213\Desktop\Documents\Project\Model\Schisto_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC830436-6231-4DED-9DD1-0B1CEADBB9C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E91900-543D-4DC5-AC12-254FF4904EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="17">
   <si>
     <t xml:space="preserve">Endemicity </t>
   </si>
@@ -79,6 +81,12 @@
   </si>
   <si>
     <t>Equilibrium</t>
+  </si>
+  <si>
+    <t>Bounce-back</t>
+  </si>
+  <si>
+    <t>Age-intensity profiles</t>
   </si>
 </sst>
 </file>
@@ -235,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -292,6 +300,7 @@
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,8 +584,8 @@
   <dimension ref="A1:XFC82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L60" sqref="L60"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J78" sqref="J78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,6 +595,8 @@
     <col min="6" max="6" width="17.44140625" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" customWidth="1"/>
     <col min="9" max="9" width="17.21875" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -616,6 +627,12 @@
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
@@ -636,8 +653,12 @@
       <c r="I2" s="54" t="b">
         <v>0</v>
       </c>
-      <c r="J2"/>
-      <c r="K2"/>
+      <c r="J2" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="54" t="b">
+        <v>0</v>
+      </c>
       <c r="L2"/>
       <c r="M2"/>
       <c r="N2"/>
@@ -680,8 +701,12 @@
       <c r="I3" t="b">
         <v>1</v>
       </c>
-      <c r="J3"/>
-      <c r="K3"/>
+      <c r="J3" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3"/>
@@ -724,8 +749,12 @@
       <c r="I4" t="b">
         <v>1</v>
       </c>
-      <c r="J4"/>
-      <c r="K4"/>
+      <c r="J4" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
       <c r="L4"/>
       <c r="M4"/>
       <c r="N4"/>
@@ -767,8 +796,12 @@
       <c r="I5" t="b">
         <v>1</v>
       </c>
-      <c r="J5"/>
-      <c r="K5"/>
+      <c r="J5" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
       <c r="L5"/>
       <c r="M5"/>
       <c r="N5"/>
@@ -810,8 +843,12 @@
       <c r="I6" t="b">
         <v>1</v>
       </c>
-      <c r="J6"/>
-      <c r="K6"/>
+      <c r="J6" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
       <c r="L6"/>
       <c r="M6"/>
       <c r="N6"/>
@@ -853,8 +890,12 @@
       <c r="I7" t="b">
         <v>1</v>
       </c>
-      <c r="J7"/>
-      <c r="K7"/>
+      <c r="J7" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
       <c r="L7"/>
       <c r="M7"/>
       <c r="N7"/>
@@ -896,8 +937,12 @@
       <c r="I8" t="b">
         <v>1</v>
       </c>
-      <c r="J8"/>
-      <c r="K8"/>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
       <c r="L8"/>
       <c r="M8"/>
       <c r="N8"/>
@@ -939,8 +984,12 @@
       <c r="I9" t="b">
         <v>1</v>
       </c>
-      <c r="J9"/>
-      <c r="K9"/>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
       <c r="L9"/>
       <c r="M9"/>
       <c r="N9"/>
@@ -982,8 +1031,12 @@
       <c r="I10" t="b">
         <v>1</v>
       </c>
-      <c r="J10"/>
-      <c r="K10"/>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
       <c r="L10"/>
       <c r="M10"/>
       <c r="N10"/>
@@ -1026,8 +1079,12 @@
       <c r="I11" t="b">
         <v>1</v>
       </c>
-      <c r="J11"/>
-      <c r="K11"/>
+      <c r="J11" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
       <c r="L11"/>
       <c r="M11"/>
       <c r="N11"/>
@@ -1070,8 +1127,12 @@
       <c r="I12" t="b">
         <v>1</v>
       </c>
-      <c r="J12"/>
-      <c r="K12"/>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
       <c r="L12"/>
       <c r="M12"/>
       <c r="N12"/>
@@ -1114,8 +1175,12 @@
       <c r="I13" t="b">
         <v>1</v>
       </c>
-      <c r="J13"/>
-      <c r="K13"/>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
       <c r="L13"/>
       <c r="M13"/>
       <c r="N13"/>
@@ -1157,8 +1222,12 @@
       <c r="I14" t="b">
         <v>1</v>
       </c>
-      <c r="J14"/>
-      <c r="K14"/>
+      <c r="J14" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
       <c r="L14"/>
       <c r="M14"/>
       <c r="N14"/>
@@ -1200,8 +1269,12 @@
       <c r="I15" t="b">
         <v>1</v>
       </c>
-      <c r="J15"/>
-      <c r="K15"/>
+      <c r="J15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" t="b">
+        <v>1</v>
+      </c>
       <c r="L15"/>
       <c r="M15"/>
       <c r="N15"/>
@@ -1243,8 +1316,12 @@
       <c r="I16" t="b">
         <v>1</v>
       </c>
-      <c r="J16"/>
-      <c r="K16"/>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" t="b">
+        <v>1</v>
+      </c>
       <c r="L16"/>
       <c r="M16"/>
       <c r="N16"/>
@@ -1286,8 +1363,12 @@
       <c r="I17" t="b">
         <v>1</v>
       </c>
-      <c r="J17"/>
-      <c r="K17"/>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="b">
+        <v>1</v>
+      </c>
       <c r="L17"/>
       <c r="M17"/>
       <c r="N17"/>
@@ -1329,8 +1410,12 @@
       <c r="I18" t="b">
         <v>1</v>
       </c>
-      <c r="J18"/>
-      <c r="K18"/>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" t="b">
+        <v>1</v>
+      </c>
       <c r="L18"/>
       <c r="M18"/>
       <c r="N18"/>
@@ -1372,8 +1457,12 @@
       <c r="I19" t="b">
         <v>1</v>
       </c>
-      <c r="J19"/>
-      <c r="K19"/>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
       <c r="L19"/>
       <c r="M19"/>
       <c r="N19"/>
@@ -1415,8 +1504,12 @@
       <c r="I20" t="b">
         <v>1</v>
       </c>
-      <c r="J20"/>
-      <c r="K20"/>
+      <c r="J20" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
       <c r="L20"/>
       <c r="M20"/>
       <c r="N20"/>
@@ -1458,8 +1551,12 @@
       <c r="I21" t="b">
         <v>1</v>
       </c>
-      <c r="J21"/>
-      <c r="K21"/>
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
       <c r="L21"/>
       <c r="M21"/>
       <c r="N21"/>
@@ -1501,8 +1598,12 @@
       <c r="I22" t="b">
         <v>1</v>
       </c>
-      <c r="J22"/>
-      <c r="K22"/>
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" t="b">
+        <v>1</v>
+      </c>
       <c r="L22"/>
       <c r="M22"/>
       <c r="N22"/>
@@ -1544,8 +1645,12 @@
       <c r="I23" t="b">
         <v>1</v>
       </c>
-      <c r="J23"/>
-      <c r="K23"/>
+      <c r="J23" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
       <c r="L23"/>
       <c r="M23"/>
       <c r="N23"/>
@@ -1587,8 +1692,12 @@
       <c r="I24" t="b">
         <v>1</v>
       </c>
-      <c r="J24"/>
-      <c r="K24"/>
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
       <c r="L24"/>
       <c r="M24"/>
       <c r="N24"/>
@@ -1630,8 +1739,12 @@
       <c r="I25" t="b">
         <v>1</v>
       </c>
-      <c r="J25"/>
-      <c r="K25"/>
+      <c r="J25" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" t="b">
+        <v>1</v>
+      </c>
       <c r="L25"/>
       <c r="M25"/>
       <c r="N25"/>
@@ -1673,8 +1786,12 @@
       <c r="I26" t="b">
         <v>1</v>
       </c>
-      <c r="J26"/>
-      <c r="K26"/>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" t="b">
+        <v>1</v>
+      </c>
       <c r="L26"/>
       <c r="M26"/>
       <c r="N26"/>
@@ -1716,8 +1833,12 @@
       <c r="I27" t="b">
         <v>1</v>
       </c>
-      <c r="J27"/>
-      <c r="K27"/>
+      <c r="J27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
+      </c>
       <c r="L27"/>
       <c r="M27"/>
       <c r="N27"/>
@@ -1759,8 +1880,12 @@
       <c r="I28" s="51" t="b">
         <v>1</v>
       </c>
-      <c r="J28"/>
-      <c r="K28"/>
+      <c r="J28" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" s="51" t="b">
+        <v>1</v>
+      </c>
       <c r="L28"/>
       <c r="M28"/>
       <c r="N28"/>
@@ -1796,6 +1921,12 @@
       <c r="I29" s="54" t="b">
         <v>0</v>
       </c>
+      <c r="J29" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="29" t="s">
@@ -1825,6 +1956,12 @@
       <c r="I30" t="b">
         <v>1</v>
       </c>
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="29" t="s">
@@ -1854,6 +1991,12 @@
       <c r="I31" t="b">
         <v>1</v>
       </c>
+      <c r="J31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="30" t="s">
@@ -1884,6 +2027,12 @@
       <c r="I32" t="b">
         <v>1</v>
       </c>
+      <c r="J32" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A33" s="30" t="s">
@@ -1914,6 +2063,12 @@
       <c r="I33" t="b">
         <v>1</v>
       </c>
+      <c r="J33" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A34" s="30" t="s">
@@ -1944,6 +2099,12 @@
       <c r="I34" t="b">
         <v>1</v>
       </c>
+      <c r="J34" t="b">
+        <v>1</v>
+      </c>
+      <c r="K34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A35" s="31" t="s">
@@ -1974,6 +2135,12 @@
       <c r="I35" t="b">
         <v>1</v>
       </c>
+      <c r="J35" t="b">
+        <v>1</v>
+      </c>
+      <c r="K35" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
@@ -2004,6 +2171,12 @@
       <c r="I36" t="b">
         <v>1</v>
       </c>
+      <c r="J36" t="b">
+        <v>1</v>
+      </c>
+      <c r="K36" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
@@ -2034,6 +2207,12 @@
       <c r="I37" t="b">
         <v>1</v>
       </c>
+      <c r="J37" t="b">
+        <v>1</v>
+      </c>
+      <c r="K37" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:16383" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="36" t="s">
@@ -2064,8 +2243,12 @@
       <c r="I38" t="b">
         <v>1</v>
       </c>
-      <c r="J38"/>
-      <c r="K38"/>
+      <c r="J38" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" t="b">
+        <v>1</v>
+      </c>
       <c r="L38"/>
       <c r="M38"/>
       <c r="N38"/>
@@ -2106,8 +2289,12 @@
       <c r="I39" t="b">
         <v>1</v>
       </c>
-      <c r="J39"/>
-      <c r="K39"/>
+      <c r="J39" t="b">
+        <v>1</v>
+      </c>
+      <c r="K39" t="b">
+        <v>1</v>
+      </c>
       <c r="L39"/>
       <c r="M39"/>
       <c r="N39"/>
@@ -2148,8 +2335,12 @@
       <c r="I40" t="b">
         <v>1</v>
       </c>
-      <c r="J40"/>
-      <c r="K40"/>
+      <c r="J40" t="b">
+        <v>1</v>
+      </c>
+      <c r="K40" t="b">
+        <v>1</v>
+      </c>
       <c r="L40"/>
       <c r="M40"/>
       <c r="N40"/>
@@ -2189,8 +2380,12 @@
       <c r="I41" t="b">
         <v>1</v>
       </c>
-      <c r="J41"/>
-      <c r="K41"/>
+      <c r="J41" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K41" t="b">
+        <v>1</v>
+      </c>
       <c r="L41"/>
       <c r="M41"/>
       <c r="N41"/>
@@ -2230,8 +2425,12 @@
       <c r="I42" t="b">
         <v>1</v>
       </c>
-      <c r="J42"/>
-      <c r="K42"/>
+      <c r="J42" t="b">
+        <v>1</v>
+      </c>
+      <c r="K42" t="b">
+        <v>1</v>
+      </c>
       <c r="L42"/>
       <c r="M42"/>
       <c r="N42"/>
@@ -2271,8 +2470,12 @@
       <c r="I43" t="b">
         <v>1</v>
       </c>
-      <c r="J43"/>
-      <c r="K43"/>
+      <c r="J43" t="b">
+        <v>1</v>
+      </c>
+      <c r="K43" t="b">
+        <v>1</v>
+      </c>
       <c r="L43"/>
       <c r="M43"/>
       <c r="N43"/>
@@ -2312,8 +2515,12 @@
       <c r="I44" t="b">
         <v>1</v>
       </c>
-      <c r="J44"/>
-      <c r="K44"/>
+      <c r="J44" t="b">
+        <v>1</v>
+      </c>
+      <c r="K44" s="54" t="b">
+        <v>0</v>
+      </c>
       <c r="L44"/>
       <c r="M44"/>
       <c r="N44"/>
@@ -2353,8 +2560,12 @@
       <c r="I45" t="b">
         <v>1</v>
       </c>
-      <c r="J45"/>
-      <c r="K45"/>
+      <c r="J45" t="b">
+        <v>1</v>
+      </c>
+      <c r="K45" s="54" t="b">
+        <v>0</v>
+      </c>
       <c r="L45"/>
       <c r="M45"/>
       <c r="N45"/>
@@ -2394,8 +2605,12 @@
       <c r="I46" t="b">
         <v>1</v>
       </c>
-      <c r="J46"/>
-      <c r="K46"/>
+      <c r="J46" t="b">
+        <v>1</v>
+      </c>
+      <c r="K46" s="54" t="b">
+        <v>0</v>
+      </c>
       <c r="L46"/>
       <c r="M46"/>
       <c r="N46"/>
@@ -2433,6 +2648,12 @@
         <v>1E-10</v>
       </c>
       <c r="I47" t="b">
+        <v>1</v>
+      </c>
+      <c r="J47" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K47" t="b">
         <v>1</v>
       </c>
       <c r="V47" s="16"/>
@@ -18826,6 +19047,12 @@
       <c r="I48" t="b">
         <v>1</v>
       </c>
+      <c r="J48" t="b">
+        <v>1</v>
+      </c>
+      <c r="K48" t="b">
+        <v>1</v>
+      </c>
       <c r="V48" s="16"/>
       <c r="W48" s="16"/>
       <c r="X48" s="16"/>
@@ -35217,6 +35444,12 @@
       <c r="I49" t="b">
         <v>1</v>
       </c>
+      <c r="J49" t="b">
+        <v>1</v>
+      </c>
+      <c r="K49" t="b">
+        <v>1</v>
+      </c>
       <c r="V49" s="16"/>
       <c r="W49" s="16"/>
       <c r="X49" s="16"/>
@@ -51608,6 +51841,12 @@
       <c r="I50" t="b">
         <v>1</v>
       </c>
+      <c r="J50" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K50" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A51" s="33" t="s">
@@ -51637,6 +51876,12 @@
       <c r="I51" t="b">
         <v>1</v>
       </c>
+      <c r="J51" t="b">
+        <v>1</v>
+      </c>
+      <c r="K51" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A52" s="33" t="s">
@@ -51666,6 +51911,12 @@
       <c r="I52" t="b">
         <v>1</v>
       </c>
+      <c r="J52" t="b">
+        <v>1</v>
+      </c>
+      <c r="K52" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A53" s="34" t="s">
@@ -51695,6 +51946,12 @@
       <c r="I53" t="b">
         <v>1</v>
       </c>
+      <c r="J53" t="b">
+        <v>1</v>
+      </c>
+      <c r="K53" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A54" s="34" t="s">
@@ -51724,6 +51981,12 @@
       <c r="I54" t="b">
         <v>1</v>
       </c>
+      <c r="J54" t="b">
+        <v>1</v>
+      </c>
+      <c r="K54" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:16383" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="35" t="s">
@@ -51753,6 +52016,12 @@
       <c r="I55" s="51" t="b">
         <v>1</v>
       </c>
+      <c r="J55" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="K55" s="56" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A56" s="28" t="s">
@@ -51782,6 +52051,12 @@
       <c r="I56" s="54" t="b">
         <v>0</v>
       </c>
+      <c r="J56" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K56" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A57" s="29" t="s">
@@ -51811,6 +52086,12 @@
       <c r="I57" s="54" t="b">
         <v>0</v>
       </c>
+      <c r="J57" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K57" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A58" s="29" t="s">
@@ -51840,6 +52121,12 @@
       <c r="I58" s="54" t="b">
         <v>0</v>
       </c>
+      <c r="J58" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K58" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A59" s="30" t="s">
@@ -51869,6 +52156,12 @@
       <c r="I59" s="54" t="b">
         <v>0</v>
       </c>
+      <c r="J59" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K59" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A60" s="30" t="s">
@@ -51898,6 +52191,12 @@
       <c r="I60" s="54" t="b">
         <v>0</v>
       </c>
+      <c r="J60" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K60" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A61" s="30" t="s">
@@ -51927,6 +52226,12 @@
       <c r="I61" s="54" t="b">
         <v>0</v>
       </c>
+      <c r="J61" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K61" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A62" s="31" t="s">
@@ -51956,6 +52261,12 @@
       <c r="I62" s="54" t="b">
         <v>0</v>
       </c>
+      <c r="J62" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K62" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A63" s="31" t="s">
@@ -51985,6 +52296,12 @@
       <c r="I63" s="54" t="b">
         <v>0</v>
       </c>
+      <c r="J63" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K63" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A64" s="31" t="s">
@@ -52014,6 +52331,12 @@
       <c r="I64" s="54" t="b">
         <v>0</v>
       </c>
+      <c r="J64" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K64" s="54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="36" t="s">
@@ -52044,8 +52367,12 @@
       <c r="I65" t="b">
         <v>1</v>
       </c>
-      <c r="J65"/>
-      <c r="K65"/>
+      <c r="J65" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K65" t="b">
+        <v>1</v>
+      </c>
       <c r="L65"/>
       <c r="M65"/>
       <c r="N65"/>
@@ -52087,8 +52414,12 @@
       <c r="I66" t="b">
         <v>1</v>
       </c>
-      <c r="J66"/>
-      <c r="K66"/>
+      <c r="J66" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K66" t="b">
+        <v>1</v>
+      </c>
       <c r="L66"/>
       <c r="M66"/>
       <c r="N66"/>
@@ -52130,8 +52461,12 @@
       <c r="I67" t="b">
         <v>1</v>
       </c>
-      <c r="J67"/>
-      <c r="K67"/>
+      <c r="J67" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K67" t="b">
+        <v>1</v>
+      </c>
       <c r="L67"/>
       <c r="M67"/>
       <c r="N67"/>
@@ -52172,8 +52507,12 @@
       <c r="I68" t="b">
         <v>1</v>
       </c>
-      <c r="J68"/>
-      <c r="K68"/>
+      <c r="J68" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K68" t="b">
+        <v>1</v>
+      </c>
       <c r="L68"/>
       <c r="M68"/>
       <c r="N68"/>
@@ -52214,8 +52553,12 @@
       <c r="I69" t="b">
         <v>1</v>
       </c>
-      <c r="J69"/>
-      <c r="K69"/>
+      <c r="J69" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K69" t="b">
+        <v>1</v>
+      </c>
       <c r="L69"/>
       <c r="M69"/>
       <c r="N69"/>
@@ -52256,8 +52599,12 @@
       <c r="I70" t="b">
         <v>1</v>
       </c>
-      <c r="J70"/>
-      <c r="K70"/>
+      <c r="J70" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K70" t="b">
+        <v>1</v>
+      </c>
       <c r="L70"/>
       <c r="M70"/>
       <c r="N70"/>
@@ -52298,8 +52645,12 @@
       <c r="I71" t="b">
         <v>1</v>
       </c>
-      <c r="J71"/>
-      <c r="K71"/>
+      <c r="J71" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K71" t="b">
+        <v>1</v>
+      </c>
       <c r="L71"/>
       <c r="M71"/>
       <c r="N71"/>
@@ -52340,8 +52691,12 @@
       <c r="I72" t="b">
         <v>1</v>
       </c>
-      <c r="J72"/>
-      <c r="K72"/>
+      <c r="J72" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K72" t="b">
+        <v>1</v>
+      </c>
       <c r="L72"/>
       <c r="M72"/>
       <c r="N72"/>
@@ -52382,8 +52737,12 @@
       <c r="I73" t="b">
         <v>1</v>
       </c>
-      <c r="J73"/>
-      <c r="K73"/>
+      <c r="J73" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K73" t="b">
+        <v>1</v>
+      </c>
       <c r="L73"/>
       <c r="M73"/>
       <c r="N73"/>
@@ -52425,6 +52784,12 @@
       <c r="I74" t="b">
         <v>1</v>
       </c>
+      <c r="J74" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K74" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A75" s="32" t="s">
@@ -52455,6 +52820,12 @@
       <c r="I75" t="b">
         <v>1</v>
       </c>
+      <c r="J75" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K75" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A76" s="32" t="s">
@@ -52485,6 +52856,12 @@
       <c r="I76" t="b">
         <v>1</v>
       </c>
+      <c r="J76" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K76" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A77" s="33" t="s">
@@ -52514,6 +52891,12 @@
       <c r="I77" t="b">
         <v>1</v>
       </c>
+      <c r="J77" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K77" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A78" s="33" t="s">
@@ -52543,6 +52926,12 @@
       <c r="I78" t="b">
         <v>1</v>
       </c>
+      <c r="J78" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K78" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A79" s="33" t="s">
@@ -52572,6 +52961,12 @@
       <c r="I79" t="b">
         <v>1</v>
       </c>
+      <c r="J79" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K79" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A80" s="34" t="s">
@@ -52601,8 +52996,14 @@
       <c r="I80" t="b">
         <v>1</v>
       </c>
+      <c r="J80" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K80" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="34" t="s">
         <v>12</v>
       </c>
@@ -52630,8 +53031,14 @@
       <c r="I81" t="b">
         <v>1</v>
       </c>
+      <c r="J81" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K81" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="82" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="35" t="s">
         <v>12</v>
       </c>
@@ -52657,6 +53064,12 @@
         <v>3.6E-9</v>
       </c>
       <c r="I82" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="J82" s="56" t="b">
+        <v>0</v>
+      </c>
+      <c r="K82" s="51" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>